<commit_message>
Fix excel on accounting module
</commit_message>
<xml_diff>
--- a/modules/accounting/uploads/file_sample/Sample_import_banking_file_en.xlsx
+++ b/modules/accounting/uploads/file_sample/Sample_import_banking_file_en.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cai dat\projects\perfexsoft_dev\modules\accounting\uploads\file_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\Root Dir\برنامج المحاماة\إضافات\المحاسبة\03-07-2021\accounting\uploads\file_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1982CC4C-CB48-4BAE-99ED-A3F94B216517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,30 +27,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>* Withdrawals</t>
+    <t>* Date (dd/mm/YYYY)</t>
   </si>
   <si>
-    <t xml:space="preserve"> * Payee</t>
+    <t xml:space="preserve"> * Payee/المستفيد</t>
   </si>
   <si>
-    <t>* Deposits</t>
+    <t>Description/الوصف</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>* Deposits/الودائع</t>
   </si>
   <si>
-    <t>* Date (dd/mm/YYYY)</t>
+    <t>* Withdrawals/السحوبات</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -127,7 +128,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,32 +405,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="33.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="5" width="33.58203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Accounting & purchase & payroll modules
</commit_message>
<xml_diff>
--- a/modules/accounting/uploads/file_sample/Sample_import_banking_file_en.xlsx
+++ b/modules/accounting/uploads/file_sample/Sample_import_banking_file_en.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\Root Dir\برنامج المحاماة\إضافات\المحاسبة\03-07-2021\accounting\uploads\file_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cai dat\projects\perfexsoft_dev\modules\accounting\uploads\file_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1982CC4C-CB48-4BAE-99ED-A3F94B216517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,30 +26,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>* Date (dd/mm/YYYY)</t>
+    <t>* Withdrawals</t>
   </si>
   <si>
-    <t xml:space="preserve"> * Payee/المستفيد</t>
+    <t xml:space="preserve"> * Payee</t>
   </si>
   <si>
-    <t>Description/الوصف</t>
+    <t>* Deposits</t>
   </si>
   <si>
-    <t>* Deposits/الودائع</t>
+    <t>Description</t>
   </si>
   <si>
-    <t>* Withdrawals/السحوبات</t>
+    <t>* Date (dd/mm/YYYY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,7 +127,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="عادي" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,34 +404,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="33.58203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="3"/>
+    <col min="1" max="5" width="33.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>